<commit_message>
Commit suite au mentorat
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\OpenClassroom\JeremyTardini_4_19072021\Starting website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB14EF8-48CB-42F3-974D-378158E72808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D26B49-05DE-4F4C-A75B-AC4D903865E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1890" windowWidth="21600" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page Index" sheetId="1" r:id="rId1"/>
-    <sheet name="Page 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Page Contact" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>Catégorie</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Multitude de lien annuaire dans le footer</t>
   </si>
   <si>
-    <t>Suppression div footer</t>
-  </si>
-  <si>
     <t>IMG ne repondant pas au exigences d'acessibilité</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>encadrement par la balise &lt;strong&gt; des keywords dans les &lt;p&gt;</t>
   </si>
   <si>
-    <t>ACCESSIBILITE</t>
-  </si>
-  <si>
     <t>réaliser des pages de 400 lignes et trié par sous repertoire le contenu</t>
   </si>
   <si>
@@ -283,17 +277,80 @@
     <t>probleme d'affichage menu</t>
   </si>
   <si>
-    <t>le menu n'est pas responsive et ne s'affiche pas coorectement</t>
-  </si>
-  <si>
     <t>corriger le css</t>
+  </si>
+  <si>
+    <t>Manque de MetaBalise</t>
+  </si>
+  <si>
+    <t>le menu n'est pas responsive et ne s'affiche pas correctement</t>
+  </si>
+  <si>
+    <t>Il n'y a aucunes Meta balise (&lt;article&gt;, &lt;footer&gt; ETC ..)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans le but d'indexer correctement les thémes de la page, toujours utiliser des métabalises </t>
+  </si>
+  <si>
+    <t>Rajout des balise Article pour définir le sujet de la pages.</t>
+  </si>
+  <si>
+    <t>Corriger les redirection vers Bootstrap et et-line.css etc …</t>
+  </si>
+  <si>
+    <t>https://www.rerp.fr/avantages-de-google-analytics-entreprise/</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/guidelines/irrelevant-keywords?__hstc=20629287.1d79d21d654290a146aa1c856fde36bd.1557946813781.1572284256555.1576603906806.8&amp;__hssc=20629287.1.1576603906806&amp;__hsfp=2220072992&amp;visit_id=637659268296394082-127720686&amp;rd=1</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/lindex-mobile-first-de-google-le-guide-complet/ ; https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055226-pensez-mobile-first</t>
+  </si>
+  <si>
+    <t>Suppression des liens dans le footer</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site</t>
+  </si>
+  <si>
+    <t>https://www.referenseo.com/blog/balise-strong-seo-referencement/</t>
+  </si>
+  <si>
+    <t>https://fiches-pratiques.chefdentreprise.com/Thematique/marketing-1052/FichePratique/Quel-est-l-interet-des-balises-semantiques--351215.htm#:~:text=C'est%20quoi%20balises%20s%C3%A9mantiques%20%3F&amp;text=Utiles%20dans%20l'optimisation%20des,du%20contenu%20qui%20est%20pr%C3%A9sent%C3%A9.</t>
+  </si>
+  <si>
+    <t>Pas de balises Robots</t>
+  </si>
+  <si>
+    <t>Impossiblite a Google bot de parcourir le site</t>
+  </si>
+  <si>
+    <t>Insérer un Balise Meta Robots</t>
+  </si>
+  <si>
+    <t>Insertion : &lt;meta name="robots" content="noindex" /&gt; dans le &lt;Head&gt;</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-technique-seo-balise-meta-robots/</t>
+  </si>
+  <si>
+    <t>SEO/ACCESSIBILITE</t>
+  </si>
+  <si>
+    <t>manque de visibilité</t>
+  </si>
+  <si>
+    <t>SEO / ACCESSIBILITE</t>
+  </si>
+  <si>
+    <t>liens morts partenaires</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,14 +399,20 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,12 +440,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,14 +708,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -681,9 +736,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -711,9 +763,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -724,7 +773,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -744,55 +792,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1011,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1009"/>
+  <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1022,734 +1071,780 @@
     <col min="1" max="1" width="21.21875" customWidth="1"/>
     <col min="2" max="2" width="25.77734375" customWidth="1"/>
     <col min="3" max="5" width="43.77734375" customWidth="1"/>
-    <col min="6" max="6" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="250.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="44"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="46"/>
+      <c r="B12" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48"/>
+      <c r="B18" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-    </row>
-    <row r="3" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="21" t="s">
+      <c r="B23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="30"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
-      <c r="B12" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:26" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="16" t="s">
+      <c r="C25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D25" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+    </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2691,18 +2786,34 @@
     <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{5BB0ECE3-B3CF-4F16-957C-83A9CF5D4D50}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{CF9A5849-550B-4DB8-B908-C9AC9E096A19}"/>
+    <hyperlink ref="F5" r:id="rId3" display="https://optimiz.me/lindex-mobile-first-de-google-le-guide-complet/ " xr:uid="{88E9BAD6-382D-4D2F-AFF9-AEFCEA491AA7}"/>
+    <hyperlink ref="F9" r:id="rId4" display="https://developers.google.com/search/docs/advanced/guidelines/irrelevant-keywords?__hstc=20629287.1d79d21d654290a146aa1c856fde36bd.1557946813781.1572284256555.1576603906806.8&amp;__hssc=20629287.1.1576603906806&amp;__hsfp=2220072992&amp;visit_id=637659268296394082-127720686&amp;rd=1" xr:uid="{93948201-8DDD-43A9-A47D-25D41F9CCB4B}"/>
+    <hyperlink ref="F14" r:id="rId5" xr:uid="{CA354E98-4BCF-4D55-9905-D6DD7B776D67}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{5B98FC5C-4ACF-440D-AD5A-013F0D9990F5}"/>
+    <hyperlink ref="F15" r:id="rId7" xr:uid="{6F34346C-4BDE-4D70-9C71-C19ED8D185F5}"/>
+    <hyperlink ref="F16" r:id="rId8" xr:uid="{77F830D8-1E5F-44AB-A87E-049456428549}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{77855E6B-E7B5-44C8-94BB-4C1E58DA49A3}"/>
+    <hyperlink ref="F7" r:id="rId10" xr:uid="{24BB8A26-0A5C-46B9-8C73-5C260403F867}"/>
+    <hyperlink ref="F6" r:id="rId11" location=":~:text=C'est%20quoi%20balises%20s%C3%A9mantiques%20%3F&amp;text=Utiles%20dans%20l'optimisation%20des,du%20contenu%20qui%20est%20pr%C3%A9sent%C3%A9." display="https://fiches-pratiques.chefdentreprise.com/Thematique/marketing-1052/FichePratique/Quel-est-l-interet-des-balises-semantiques--351215.htm#:~:text=C'est%20quoi%20balises%20s%C3%A9mantiques%20%3F&amp;text=Utiles%20dans%20l'optimisation%20des,du%20contenu%20qui%20est%20pr%C3%A9sent%C3%A9." xr:uid="{E5442813-6901-4E59-9546-F00FFACDD6CD}"/>
+    <hyperlink ref="F11" r:id="rId12" xr:uid="{B2220D41-942B-427E-8689-EC6C9DA4B56C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA310B4F-9D60-45CF-98D9-28B8FF03292C}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2713,259 +2824,189 @@
     <col min="6" max="6" width="67.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="48"/>
+      <c r="B6" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="49"/>
+    </row>
+    <row r="7" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="49"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="31"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="31"/>
+    </row>
+    <row r="10" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="32"/>
+    </row>
+    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="45"/>
-    </row>
-    <row r="3" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="26"/>
-    </row>
-    <row r="5" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="26"/>
-    </row>
-    <row r="7" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="26"/>
-    </row>
-    <row r="10" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="26"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="44"/>
-    </row>
-    <row r="12" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="54"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="41"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="27"/>
-    </row>
-    <row r="15" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16" spans="1:6" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="28"/>
-    </row>
-    <row r="17" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="55"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="35"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="35"/>
-    </row>
-    <row r="20" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="36"/>
-    </row>
-    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="34"/>
-    </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="B12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="26"/>
-    </row>
-    <row r="23" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="16" t="s">
+      <c r="B13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="28"/>
+      <c r="F13" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>